<commit_message>
All project files and data upload.
</commit_message>
<xml_diff>
--- a/patients_data.xlsx
+++ b/patients_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -26,13 +26,19 @@
     <t>Disease</t>
   </si>
   <si>
-    <t>Hussien</t>
+    <t>Mahmoud</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Flu</t>
+    <t>Oseogenesis</t>
+  </si>
+  <si>
+    <t>Hesham</t>
+  </si>
+  <si>
+    <t>Headache</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -97,6 +103,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>